<commit_message>
actualitzar inferencia 3 funcions josep i arnau filtrar per dificultat
</commit_message>
<xml_diff>
--- a/exercices_to_clips/exercicisExcel.xlsx
+++ b/exercices_to_clips/exercicisExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="247">
   <si>
     <t>nom_instancia</t>
   </si>
@@ -144,12 +144,18 @@
     <t>Facil</t>
   </si>
   <si>
+    <t>MusculacioMantenimentPosar_se_en_forma</t>
+  </si>
+  <si>
     <t>jalon_al_pecho</t>
   </si>
   <si>
     <t>jalon al pecho</t>
   </si>
   <si>
+    <t>MusculacioPosar_se_en_forma</t>
+  </si>
+  <si>
     <t>remo_gironda</t>
   </si>
   <si>
@@ -171,6 +177,9 @@
     <t>Mitja</t>
   </si>
   <si>
+    <t>MusculacioManteniment</t>
+  </si>
+  <si>
     <t>extension_cuadriceps</t>
   </si>
   <si>
@@ -186,7 +195,10 @@
     <t>sentadilla</t>
   </si>
   <si>
-    <t>hack</t>
+    <t>hack_squat</t>
+  </si>
+  <si>
+    <t>hack squat</t>
   </si>
   <si>
     <t>abductores</t>
@@ -336,12 +348,18 @@
     <t>saltar a la comba</t>
   </si>
   <si>
+    <t>Baixar_de_pesMantenimentPosar_se_en_forma</t>
+  </si>
+  <si>
     <t>aqua_gym</t>
   </si>
   <si>
     <t>aqua gym</t>
   </si>
   <si>
+    <t>Baixar_de_pesManteniment</t>
+  </si>
+  <si>
     <t>idas_y_vueltas_piscina</t>
   </si>
   <si>
@@ -411,6 +429,9 @@
     <t>zancadas patinador</t>
   </si>
   <si>
+    <t>Baixar_de_pesPosar_se_en_forma</t>
+  </si>
+  <si>
     <t>rollbacks</t>
   </si>
   <si>
@@ -507,6 +528,9 @@
     <t>estiramiento cuello</t>
   </si>
   <si>
+    <t>RehabilitacioManteniment</t>
+  </si>
+  <si>
     <t>balanceo_con_kettlebell</t>
   </si>
   <si>
@@ -691,6 +715,48 @@
   </si>
   <si>
     <t>estiramiento de cuello</t>
+  </si>
+  <si>
+    <t>postura_del_gato</t>
+  </si>
+  <si>
+    <t>postura del gato</t>
+  </si>
+  <si>
+    <t>postura_del_niño</t>
+  </si>
+  <si>
+    <t>postura del niño</t>
+  </si>
+  <si>
+    <t>estiramiento_de_mariposa</t>
+  </si>
+  <si>
+    <t>estiramiento de mariposa</t>
+  </si>
+  <si>
+    <t>EsquenaBraç</t>
+  </si>
+  <si>
+    <t>estiramiento_de_isquiotibiales_en_pie</t>
+  </si>
+  <si>
+    <t>estiramiento triceps</t>
+  </si>
+  <si>
+    <t>postura_del_camello</t>
+  </si>
+  <si>
+    <t>postura del camello</t>
+  </si>
+  <si>
+    <t>postura_de_la_paloma</t>
+  </si>
+  <si>
+    <t>postura de la paloma</t>
+  </si>
+  <si>
+    <t>EsquenaCama</t>
   </si>
 </sst>
 </file>
@@ -700,7 +766,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -715,11 +781,6 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -748,7 +809,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -759,12 +820,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -780,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -791,27 +846,18 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1030,8 +1076,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.13"/>
-    <col customWidth="1" min="2" max="2" width="23.63"/>
+    <col customWidth="1" min="1" max="1" width="29.13"/>
+    <col customWidth="1" min="2" max="2" width="29.38"/>
     <col customWidth="1" min="3" max="3" width="19.13"/>
     <col customWidth="1" min="4" max="4" width="22.13"/>
     <col customWidth="1" min="5" max="5" width="13.75"/>
@@ -1222,13 +1268,13 @@
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="5" t="b">
+      <c r="C15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1253,15 +1299,15 @@
         <v>23</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>
@@ -1288,16 +1334,16 @@
         <f>L7</f>
         <v>Esquena</v>
       </c>
-      <c r="N16" s="6" t="s">
-        <v>30</v>
+      <c r="N16" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
@@ -1327,15 +1373,15 @@
         <f>N7</f>
         <v>Musculacio</v>
       </c>
-      <c r="O17" s="7"/>
-      <c r="P17" s="8"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="7"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
@@ -1356,23 +1402,23 @@
         <v>70.0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L18" s="1" t="str">
         <f>L7</f>
         <v>Esquena</v>
       </c>
       <c r="N18" s="1" t="str">
-        <f>N7</f>
-        <v>Musculacio</v>
+        <f>N7&amp;N8</f>
+        <v>MusculacioPosar_se_en_forma</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
@@ -1393,7 +1439,7 @@
         <v>65.0</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L19" s="1" t="str">
         <f>L7</f>
@@ -1402,17 +1448,16 @@
       <c r="M19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="1" t="str">
-        <f>N7</f>
-        <v>Musculacio</v>
+      <c r="N19" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
@@ -1439,18 +1484,17 @@
         <f>L5</f>
         <v>Cama</v>
       </c>
-      <c r="N20" s="1" t="str">
-        <f>N7</f>
-        <v>Musculacio</v>
-      </c>
-      <c r="P20" s="9"/>
+      <c r="N20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>0</v>
@@ -1471,23 +1515,23 @@
         <v>70.0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L21" s="1" t="str">
         <f>L5</f>
         <v>Cama</v>
       </c>
       <c r="N21" s="1" t="str">
-        <f>N7</f>
-        <v>Musculacio</v>
+        <f>N7&amp;N8</f>
+        <v>MusculacioPosar_se_en_forma</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>0</v>
@@ -1519,10 +1563,10 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>0</v>
@@ -1543,21 +1587,21 @@
         <v>65.0</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>57</v>
+      <c r="A24" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>0</v>
@@ -1589,10 +1633,10 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>0</v>
@@ -1619,15 +1663,15 @@
         <v>25</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="b">
         <v>0</v>
@@ -1648,23 +1692,23 @@
         <v>70.0</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L26" s="1" t="str">
         <f>L8</f>
         <v>Pit</v>
       </c>
       <c r="N26" s="1" t="str">
-        <f>N7</f>
-        <v>Musculacio</v>
+        <f>N7&amp;N8</f>
+        <v>MusculacioPosar_se_en_forma</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2" t="b">
         <v>0</v>
@@ -1698,10 +1742,10 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2" t="b">
         <v>0</v>
@@ -1733,10 +1777,10 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="b">
         <v>0</v>
@@ -1757,21 +1801,21 @@
         <v>65.0</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>31</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C30" s="2" t="b">
         <v>0</v>
@@ -1798,15 +1842,15 @@
         <v>25</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C31" s="2" t="b">
         <v>0</v>
@@ -1827,7 +1871,7 @@
         <v>75.0</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>27</v>
@@ -1838,10 +1882,10 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C32" s="2" t="b">
         <v>0</v>
@@ -1868,15 +1912,15 @@
         <v>27</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C33" s="2" t="b">
         <v>0</v>
@@ -1903,15 +1947,15 @@
         <v>27</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C34" s="2" t="b">
         <v>0</v>
@@ -1920,7 +1964,7 @@
         <v>40</v>
       </c>
       <c r="G34" s="2">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="H34" s="2">
         <v>6.0</v>
@@ -1932,7 +1976,7 @@
         <v>75.0</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>27</v>
@@ -1943,10 +1987,10 @@
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C35" s="2" t="b">
         <v>0</v>
@@ -1978,10 +2022,10 @@
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C36" s="2" t="b">
         <v>0</v>
@@ -2008,15 +2052,15 @@
         <v>34</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2" t="b">
         <v>0</v>
@@ -2037,27 +2081,27 @@
         <v>75.0</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E38" s="2">
         <v>4.0</v>
@@ -2071,7 +2115,7 @@
         <v>75.0</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>34</v>
@@ -2081,11 +2125,11 @@
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="10" t="s">
-        <v>87</v>
+      <c r="A39" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C39" s="2" t="b">
         <v>0</v>
@@ -2106,21 +2150,21 @@
         <v>70.0</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="11" t="s">
-        <v>89</v>
+      <c r="A40" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C40" s="2" t="b">
         <v>0</v>
@@ -2141,21 +2185,21 @@
         <v>75.0</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="11" t="s">
-        <v>90</v>
+      <c r="A41" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C41" s="2" t="b">
         <v>0</v>
@@ -2182,15 +2226,15 @@
         <v>23</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="11" t="s">
-        <v>92</v>
+      <c r="A42" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C42" s="2" t="b">
         <v>0</v>
@@ -2211,21 +2255,21 @@
         <v>80.0</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="11" t="s">
-        <v>94</v>
+      <c r="A43" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C43" s="2" t="b">
         <v>0</v>
@@ -2252,15 +2296,15 @@
         <v>23</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="11" t="s">
-        <v>96</v>
+      <c r="A44" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C44" s="2" t="b">
         <v>0</v>
@@ -2287,15 +2331,15 @@
         <v>23</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C45" s="2" t="b">
         <v>0</v>
@@ -2316,10 +2360,10 @@
         <v>70.0</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>30</v>
@@ -2333,21 +2377,21 @@
     <row r="49" ht="12.75" customHeight="1"/>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C51" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E51" s="2">
         <v>5.0</v>
@@ -2367,22 +2411,22 @@
         <v>Cama</v>
       </c>
       <c r="N51" s="1" t="str">
-        <f>N4&amp;N8</f>
-        <v>Baixar_de_pesPosar_se_en_forma</v>
+        <f>N4&amp;N8&amp;N6</f>
+        <v>Baixar_de_pesPosar_se_en_formaManteniment</v>
       </c>
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C52" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E52" s="2">
         <v>2.0</v>
@@ -2406,21 +2450,21 @@
         <v/>
       </c>
       <c r="N52" s="2" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C53" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E53" s="2">
         <v>30.0</v>
@@ -2444,15 +2488,15 @@
         <v>BraçCamaTors</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C54" s="2" t="b">
         <v>1</v>
@@ -2473,7 +2517,7 @@
         <v>80.0</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L54" s="1" t="str">
         <f>L4&amp;L5&amp;L7</f>
@@ -2484,16 +2528,16 @@
         <v/>
       </c>
       <c r="N54" s="1" t="str">
-        <f>N4&amp;N10</f>
-        <v>Baixar_de_pes</v>
+        <f>N4&amp;N10&amp;N6</f>
+        <v>Baixar_de_pesManteniment</v>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="6" t="s">
-        <v>110</v>
+      <c r="A55" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C55" s="2" t="b">
         <v>1</v>
@@ -2526,11 +2570,11 @@
       </c>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="12" t="s">
-        <v>111</v>
+      <c r="A56" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C56" s="2" t="b">
         <v>1</v>
@@ -2551,7 +2595,7 @@
         <v>65.0</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L56" s="1" t="str">
         <f>L9&amp;L4</f>
@@ -2564,16 +2608,16 @@
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C57" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E57" s="2">
         <v>10.0</v>
@@ -2597,22 +2641,22 @@
         <v>Cama</v>
       </c>
       <c r="N57" s="1" t="str">
-        <f>N4</f>
-        <v>Baixar_de_pes</v>
+        <f>N4&amp;N6</f>
+        <v>Baixar_de_pesManteniment</v>
       </c>
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C58" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E58" s="2">
         <v>10.0</v>
@@ -2625,27 +2669,27 @@
         <v>85.0</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C59" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E59" s="2">
         <v>10.0</v>
@@ -2664,21 +2708,21 @@
         <v>25</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C60" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E60" s="2">
         <v>2.0</v>
@@ -2691,7 +2735,7 @@
         <v>80.0</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L60" s="1" t="str">
         <f>L7&amp;L4&amp;L6</f>
@@ -2701,21 +2745,21 @@
         <v>29</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C61" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E61" s="2">
         <v>1.0</v>
@@ -2728,7 +2772,7 @@
         <v>75.0</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>25</v>
@@ -2739,16 +2783,16 @@
     </row>
     <row r="62" ht="12.75" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C62" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E62" s="2">
         <v>1.0</v>
@@ -2761,7 +2805,7 @@
         <v>65.0</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>34</v>
@@ -2772,10 +2816,10 @@
     </row>
     <row r="63" ht="12.75" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2" t="b">
         <v>1</v>
@@ -2807,10 +2851,10 @@
     </row>
     <row r="64" ht="12.75" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C64" s="2" t="b">
         <v>1</v>
@@ -2837,15 +2881,15 @@
         <v>34</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C65" s="2" t="b">
         <v>1</v>
@@ -2866,7 +2910,7 @@
         <v>70.0</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>34</v>
@@ -2877,10 +2921,10 @@
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C66" s="2" t="b">
         <v>1</v>
@@ -2901,21 +2945,21 @@
         <v>70.0</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C67" s="2" t="b">
         <v>1</v>
@@ -2936,7 +2980,7 @@
         <v>70.0</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>34</v>
@@ -2947,10 +2991,10 @@
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C68" s="2" t="b">
         <v>1</v>
@@ -2977,34 +3021,34 @@
         <v>25</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C69" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E69" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F69" s="2">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="G69" s="2"/>
       <c r="J69" s="2">
         <v>65.0</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>34</v>
@@ -3015,22 +3059,22 @@
     </row>
     <row r="70" ht="12.75" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C70" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E70" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F70" s="2">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="G70" s="2"/>
       <c r="J70" s="2">
@@ -3040,37 +3084,37 @@
         <v>41</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C71" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E71" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F71" s="2">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="G71" s="2"/>
       <c r="J71" s="2">
         <v>70.0</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>25</v>
@@ -3081,29 +3125,29 @@
     </row>
     <row r="72" ht="12.75" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C72" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E72" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F72" s="2">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="G72" s="2"/>
       <c r="J72" s="2">
         <v>70.0</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>25</v>
@@ -3114,10 +3158,10 @@
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C73" s="2" t="b">
         <v>1</v>
@@ -3149,29 +3193,29 @@
     </row>
     <row r="74" ht="12.75" customHeight="1">
       <c r="A74" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C74" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E74" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F74" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="G74" s="2"/>
       <c r="J74" s="2">
         <v>70.0</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>34</v>
@@ -3182,19 +3226,19 @@
     </row>
     <row r="75" ht="12.75" customHeight="1">
       <c r="A75" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C75" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E75" s="2">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F75" s="2">
         <v>4.0</v>
@@ -3211,24 +3255,24 @@
         <v>Braç</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" ht="12.75" customHeight="1">
       <c r="A76" s="2" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C76" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E76" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F76" s="2">
         <v>3.0</v>
@@ -3238,7 +3282,7 @@
         <v>70.0</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>34</v>
@@ -3249,43 +3293,43 @@
     </row>
     <row r="77" ht="12.75" customHeight="1">
       <c r="A77" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C77" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E77" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F77" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G77" s="2"/>
       <c r="J77" s="2">
         <v>75.0</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>24</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" ht="12.75" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C78" s="2" t="b">
         <v>1</v>
@@ -3312,37 +3356,37 @@
         <v>25</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" ht="12.75" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="C79" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E79" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F79" s="2">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="G79" s="2"/>
       <c r="J79" s="2">
         <v>75.0</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="N79" s="2" t="s">
         <v>24</v>
@@ -3350,22 +3394,22 @@
     </row>
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C80" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E80" s="2">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="F80" s="2">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="G80" s="2"/>
       <c r="J80" s="2">
@@ -3378,40 +3422,40 @@
         <v>25</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" ht="12.75" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="C81" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E81" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F81" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G81" s="2"/>
       <c r="J81" s="2">
         <v>75.0</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" ht="12.75" customHeight="1"/>
@@ -3419,27 +3463,27 @@
     <row r="84" ht="12.75" customHeight="1"/>
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" s="3" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="86" ht="12.75" customHeight="1">
       <c r="A86" s="3" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C86" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E86" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="F86" s="2">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G86" s="2"/>
       <c r="J86" s="2">
@@ -3455,34 +3499,34 @@
         <v>34</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C87" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E87" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="F87" s="2">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G87" s="2"/>
       <c r="J87" s="2">
         <v>80.0</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L87" s="2" t="s">
         <v>34</v>
@@ -3496,22 +3540,22 @@
     </row>
     <row r="88" ht="12.75" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E88" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F88" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G88" s="2"/>
       <c r="J88" s="2">
@@ -3532,10 +3576,10 @@
     </row>
     <row r="89" ht="12.75" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="C89" s="2" t="b">
         <v>0</v>
@@ -3570,10 +3614,10 @@
     </row>
     <row r="90" ht="12.75" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C90" s="2" t="b">
         <v>0</v>
@@ -3594,7 +3638,7 @@
         <v>80.0</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L90" s="2" t="s">
         <v>27</v>
@@ -3608,10 +3652,10 @@
     </row>
     <row r="91" ht="12.75" customHeight="1">
       <c r="A91" s="3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C91" s="2" t="b">
         <v>0</v>
@@ -3646,10 +3690,10 @@
     </row>
     <row r="92" ht="12.75" customHeight="1">
       <c r="A92" s="3" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C92" s="2" t="b">
         <v>0</v>
@@ -3670,7 +3714,7 @@
         <v>80.0</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>27</v>
@@ -3684,22 +3728,22 @@
     </row>
     <row r="93" ht="12.75" customHeight="1">
       <c r="A93" s="2" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C93" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E93" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F93" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G93" s="2"/>
       <c r="J93" s="2">
@@ -3720,22 +3764,22 @@
     </row>
     <row r="94" ht="12.75" customHeight="1">
       <c r="A94" s="3" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C94" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E94" s="2">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="F94" s="2">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G94" s="2"/>
       <c r="J94" s="2">
@@ -3756,10 +3800,10 @@
     </row>
     <row r="95" ht="12.75" customHeight="1">
       <c r="A95" s="3" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C95" s="2" t="b">
         <v>0</v>
@@ -3789,15 +3833,15 @@
         <v>25</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" ht="12.75" customHeight="1">
       <c r="A96" s="3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C96" s="2" t="b">
         <v>0</v>
@@ -3832,10 +3876,10 @@
     </row>
     <row r="97" ht="12.75" customHeight="1">
       <c r="A97" s="3" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C97" s="2" t="b">
         <v>0</v>
@@ -3856,7 +3900,7 @@
         <v>80.0</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>25</v>
@@ -3870,28 +3914,28 @@
     </row>
     <row r="98" ht="12.75" customHeight="1">
       <c r="A98" s="3" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C98" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E98" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F98" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J98" s="2">
         <v>75.0</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>34</v>
@@ -3905,10 +3949,10 @@
     </row>
     <row r="99" ht="12.75" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C99" s="2" t="b">
         <v>0</v>
@@ -3929,7 +3973,7 @@
         <v>80.0</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>25</v>
@@ -3943,22 +3987,22 @@
     </row>
     <row r="100" ht="12.75" customHeight="1">
       <c r="A100" s="3" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="C100" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E100" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F100" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G100" s="2"/>
       <c r="J100" s="2">
@@ -3979,29 +4023,29 @@
     </row>
     <row r="101" ht="12.75" customHeight="1">
       <c r="A101" s="3" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C101" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E101" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F101" s="2">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G101" s="2"/>
       <c r="J101" s="2">
         <v>75.0</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>31</v>
@@ -4015,22 +4059,22 @@
     </row>
     <row r="102" ht="12.75" customHeight="1">
       <c r="A102" s="3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C102" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E102" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F102" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="G102" s="2"/>
       <c r="J102" s="2">
@@ -4051,29 +4095,29 @@
     </row>
     <row r="103" ht="12.75" customHeight="1">
       <c r="A103" s="3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="C103" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E103" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F103" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="G103" s="2"/>
       <c r="J103" s="2">
         <v>80.0</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>23</v>
@@ -4087,29 +4131,29 @@
     </row>
     <row r="104" ht="12.75" customHeight="1">
       <c r="A104" s="3" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C104" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E104" s="2">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="F104" s="2">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="G104" s="2"/>
       <c r="J104" s="2">
         <v>75.0</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L104" s="2" t="s">
         <v>29</v>
@@ -4118,15 +4162,15 @@
         <v>29</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" ht="12.75" customHeight="1">
       <c r="A105" s="3" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="C105" s="2" t="b">
         <v>0</v>
@@ -4161,10 +4205,10 @@
     </row>
     <row r="106" ht="12.75" customHeight="1">
       <c r="A106" s="3" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C106" s="2" t="b">
         <v>0</v>
@@ -4185,7 +4229,7 @@
         <v>75.0</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>34</v>
@@ -4199,16 +4243,16 @@
     </row>
     <row r="107" ht="12.75" customHeight="1">
       <c r="A107" s="3" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C107" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E107" s="2">
         <v>20.0</v>
@@ -4224,47 +4268,47 @@
         <v>41</v>
       </c>
       <c r="L107" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="M107" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>35</v>
+        <v>170</v>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1"/>
     <row r="109" ht="12.75" customHeight="1"/>
     <row r="110" ht="12.75" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" ht="12.75" customHeight="1">
       <c r="A111" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>208</v>
+        <v>215</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="C111" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E111" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="F111" s="2">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="G111" s="2"/>
       <c r="J111" s="2">
         <v>80.0</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>29</v>
@@ -4274,23 +4318,23 @@
       </c>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>210</v>
+      <c r="A112" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="C112" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E112" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F112" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G112" s="2"/>
       <c r="J112" s="2">
@@ -4307,23 +4351,23 @@
       </c>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B113" s="6" t="s">
-        <v>212</v>
+      <c r="A113" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="C113" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E113" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F113" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G113" s="2"/>
       <c r="J113" s="2">
@@ -4340,23 +4384,23 @@
       </c>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="6" t="s">
-        <v>213</v>
+      <c r="A114" s="5" t="s">
+        <v>221</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C114" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E114" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F114" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G114" s="2"/>
       <c r="J114" s="2">
@@ -4373,23 +4417,23 @@
       </c>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>216</v>
+      <c r="A115" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="C115" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E115" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F115" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G115" s="2"/>
       <c r="J115" s="2">
@@ -4406,30 +4450,30 @@
       </c>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="B116" s="6" t="s">
-        <v>218</v>
+      <c r="A116" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>226</v>
       </c>
       <c r="C116" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E116" s="2">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F116" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G116" s="2"/>
       <c r="J116" s="2">
         <v>80.0</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L116" s="2" t="s">
         <v>29</v>
@@ -4439,23 +4483,23 @@
       </c>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>220</v>
+      <c r="A117" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>228</v>
       </c>
       <c r="C117" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E117" s="2">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="F117" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="G117" s="2"/>
       <c r="J117" s="2">
@@ -4472,30 +4516,30 @@
       </c>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>222</v>
+      <c r="A118" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="C118" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E118" s="2">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F118" s="2">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="G118" s="2"/>
       <c r="J118" s="2">
         <v>80.0</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L118" s="2" t="s">
         <v>34</v>
@@ -4506,22 +4550,22 @@
     </row>
     <row r="119" ht="12.75" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="C119" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E119" s="2">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="F119" s="2">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="G119" s="2"/>
       <c r="J119" s="2">
@@ -4538,19 +4582,232 @@
       </c>
     </row>
     <row r="120" ht="12.75" customHeight="1">
+      <c r="A120" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C120" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E120" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F120" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="J120" s="2">
+        <v>75.0</v>
+      </c>
+      <c r="K120" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L120" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M120" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="N120" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="121" ht="12.75" customHeight="1">
-      <c r="A121" s="2"/>
-      <c r="N121" s="2"/>
-    </row>
-    <row r="122" ht="12.75" customHeight="1"/>
-    <row r="123" ht="12.75" customHeight="1"/>
-    <row r="124" ht="12.75" customHeight="1"/>
-    <row r="125" ht="12.75" customHeight="1"/>
-    <row r="126" ht="12.75" customHeight="1"/>
+      <c r="A121" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C121" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E121" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="F121" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="J121" s="2">
+        <v>75.0</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L121" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N121" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="122" ht="12.75" customHeight="1">
+      <c r="A122" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C122" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E122" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F122" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="J122" s="2">
+        <v>80.0</v>
+      </c>
+      <c r="K122" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="N122" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="123" ht="12.75" customHeight="1">
+      <c r="A123" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C123" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E123" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F123" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="J123" s="2">
+        <v>80.0</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N123" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="124" ht="12.75" customHeight="1">
+      <c r="A124" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C124" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E124" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="F124" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="J124" s="2">
+        <v>75.0</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N124" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="125" ht="12.75" customHeight="1">
+      <c r="A125" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C125" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E125" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F125" s="2">
+        <v>9.0</v>
+      </c>
+      <c r="J125" s="2">
+        <v>70.0</v>
+      </c>
+      <c r="K125" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N125" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="126" ht="12.75" customHeight="1">
+      <c r="A126" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C126" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E126" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="F126" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="J126" s="2">
+        <v>65.0</v>
+      </c>
+      <c r="K126" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L126" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="N126" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="127" ht="12.75" customHeight="1"/>
     <row r="128" ht="12.75" customHeight="1"/>
     <row r="129" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
afegir filtrar per dificultat i assinar duracio o repeticio segons intensitat
</commit_message>
<xml_diff>
--- a/exercices_to_clips/exercicisExcel.xlsx
+++ b/exercices_to_clips/exercicisExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="251">
   <si>
     <t>nom_instancia</t>
   </si>
@@ -126,6 +126,9 @@
     <t>Rehabilitacio</t>
   </si>
   <si>
+    <t>Yoga</t>
+  </si>
+  <si>
     <t>#primer(el que treballa) altres involucra</t>
   </si>
   <si>
@@ -252,6 +255,9 @@
     <t>elevaciones frontales manc</t>
   </si>
   <si>
+    <t>EspatllaBraç</t>
+  </si>
+  <si>
     <t>elevaciones_laterales</t>
   </si>
   <si>
@@ -405,6 +411,9 @@
     <t>mountain climbers</t>
   </si>
   <si>
+    <t>Baixar_de_pesPosar_se_en_forma</t>
+  </si>
+  <si>
     <t>pasos_laterales</t>
   </si>
   <si>
@@ -429,7 +438,7 @@
     <t>zancadas patinador</t>
   </si>
   <si>
-    <t>Baixar_de_pesPosar_se_en_forma</t>
+    <t>Baixar_de_pesPosar_se_en_formaManteniment</t>
   </si>
   <si>
     <t>rollbacks</t>
@@ -528,63 +537,69 @@
     <t>estiramiento cuello</t>
   </si>
   <si>
+    <t>RehabilitacioMantenimentYogaFlexibilitat</t>
+  </si>
+  <si>
+    <t>balanceo_con_kettlebell</t>
+  </si>
+  <si>
+    <t>balanceo con kettlebell</t>
+  </si>
+  <si>
+    <t>rotaciones_hombros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotaciones hombros </t>
+  </si>
+  <si>
+    <t>RehabilitacioYoga</t>
+  </si>
+  <si>
+    <t>elevacion_hombros</t>
+  </si>
+  <si>
+    <t>elevacion de hombros</t>
+  </si>
+  <si>
+    <t>retraimiento_escapular</t>
+  </si>
+  <si>
+    <t>retraimiento escapular</t>
+  </si>
+  <si>
+    <t>rotacion_externa_hombro</t>
+  </si>
+  <si>
+    <t>rotacion externa de hombro</t>
+  </si>
+  <si>
+    <t>abduccion_hombro</t>
+  </si>
+  <si>
+    <t>abducción de hombro</t>
+  </si>
+  <si>
+    <t>estiramiento_cuadriceps</t>
+  </si>
+  <si>
+    <t>estiramiento de cuadriceps</t>
+  </si>
+  <si>
+    <t>estiramiento_isquiotibiales</t>
+  </si>
+  <si>
+    <t>estiramiento de isquiotibiales</t>
+  </si>
+  <si>
+    <t>puente_gluteo</t>
+  </si>
+  <si>
+    <t>puente de gluteos</t>
+  </si>
+  <si>
     <t>RehabilitacioManteniment</t>
   </si>
   <si>
-    <t>balanceo_con_kettlebell</t>
-  </si>
-  <si>
-    <t>balanceo con kettlebell</t>
-  </si>
-  <si>
-    <t>rotaciones_hombros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rotaciones hombros </t>
-  </si>
-  <si>
-    <t>elevacion_hombros</t>
-  </si>
-  <si>
-    <t>elevacion de hombros</t>
-  </si>
-  <si>
-    <t>retraimiento_escapular</t>
-  </si>
-  <si>
-    <t>retraimiento escapular</t>
-  </si>
-  <si>
-    <t>rotacion_externa_hombro</t>
-  </si>
-  <si>
-    <t>rotacion externa de hombro</t>
-  </si>
-  <si>
-    <t>abduccion_hombro</t>
-  </si>
-  <si>
-    <t>abducción de hombro</t>
-  </si>
-  <si>
-    <t>estiramiento_cuadriceps</t>
-  </si>
-  <si>
-    <t>estiramiento de cuadriceps</t>
-  </si>
-  <si>
-    <t>estiramiento_isquiotibiales</t>
-  </si>
-  <si>
-    <t>estiramiento de isquiotibiales</t>
-  </si>
-  <si>
-    <t>puente_gluteo</t>
-  </si>
-  <si>
-    <t>puente de gluteos</t>
-  </si>
-  <si>
     <t>extensiones_tobillo</t>
   </si>
   <si>
@@ -660,7 +675,7 @@
     <t>BraçCamaTors</t>
   </si>
   <si>
-    <t># Flexibilitat</t>
+    <t># Flexibilitat i Yoga</t>
   </si>
   <si>
     <t>postura_de_la_cobra</t>
@@ -669,6 +684,9 @@
     <t>postura de la cobra</t>
   </si>
   <si>
+    <t>FlexibilitatYoga</t>
+  </si>
+  <si>
     <t>estiramiento_piernas</t>
   </si>
   <si>
@@ -711,10 +729,13 @@
     <t>giro torso sobre suelo</t>
   </si>
   <si>
-    <t>estiramiento_de_cuello</t>
-  </si>
-  <si>
-    <t>estiramiento de cuello</t>
+    <t>postura_de_la_paloma</t>
+  </si>
+  <si>
+    <t>postura de la paloma</t>
+  </si>
+  <si>
+    <t>EsquenaCama</t>
   </si>
   <si>
     <t>postura_del_gato</t>
@@ -748,15 +769,6 @@
   </si>
   <si>
     <t>postura del camello</t>
-  </si>
-  <si>
-    <t>postura_de_la_paloma</t>
-  </si>
-  <si>
-    <t>postura de la paloma</t>
-  </si>
-  <si>
-    <t>EsquenaCama</t>
   </si>
 </sst>
 </file>
@@ -1250,35 +1262,39 @@
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="2"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="L12" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G15" s="2">
         <v>9.0</v>
@@ -1293,27 +1309,27 @@
         <v>75.0</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2">
         <v>12.0</v>
@@ -1328,28 +1344,28 @@
         <v>75.0</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L16" s="1" t="str">
         <f>L7</f>
         <v>Esquena</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G17" s="2">
         <v>10.0</v>
@@ -1364,7 +1380,7 @@
         <v>75.0</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>29</v>
@@ -1378,16 +1394,16 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G18" s="2">
         <v>10.0</v>
@@ -1402,7 +1418,7 @@
         <v>70.0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L18" s="1" t="str">
         <f>L7</f>
@@ -1415,16 +1431,16 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G19" s="2">
         <v>8.0</v>
@@ -1439,7 +1455,7 @@
         <v>65.0</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L19" s="1" t="str">
         <f>L7</f>
@@ -1449,21 +1465,21 @@
         <v>29</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G20" s="2">
         <v>9.0</v>
@@ -1478,29 +1494,29 @@
         <v>80.0</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L20" s="1" t="str">
         <f>L5</f>
         <v>Cama</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P20" s="8"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G21" s="2">
         <v>12.0</v>
@@ -1515,7 +1531,7 @@
         <v>70.0</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L21" s="1" t="str">
         <f>L5</f>
@@ -1528,16 +1544,16 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G22" s="2">
         <v>10.0</v>
@@ -1552,7 +1568,7 @@
         <v>70.0</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>25</v>
@@ -1563,16 +1579,16 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G23" s="2">
         <v>10.0</v>
@@ -1587,27 +1603,27 @@
         <v>65.0</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G24" s="2">
         <v>8.0</v>
@@ -1622,7 +1638,7 @@
         <v>80.0</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>25</v>
@@ -1633,16 +1649,16 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G25" s="2">
         <v>6.0</v>
@@ -1657,27 +1673,27 @@
         <v>85.0</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G26" s="2">
         <v>9.0</v>
@@ -1692,7 +1708,7 @@
         <v>70.0</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L26" s="1" t="str">
         <f>L8</f>
@@ -1705,16 +1721,16 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G27" s="2">
         <v>10.0</v>
@@ -1729,7 +1745,7 @@
         <v>75.0</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L27" s="1" t="str">
         <f>L8</f>
@@ -1742,16 +1758,16 @@
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G28" s="2">
         <v>8.0</v>
@@ -1766,7 +1782,7 @@
         <v>70.0</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>31</v>
@@ -1777,16 +1793,16 @@
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G29" s="2">
         <v>13.0</v>
@@ -1801,27 +1817,27 @@
         <v>65.0</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>31</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G30" s="2">
         <v>10.0</v>
@@ -1836,27 +1852,27 @@
         <v>75.0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C31" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G31" s="2">
         <v>10.0</v>
@@ -1871,7 +1887,7 @@
         <v>75.0</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>27</v>
@@ -1882,16 +1898,16 @@
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G32" s="2">
         <v>8.0</v>
@@ -1906,27 +1922,27 @@
         <v>75.0</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C33" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G33" s="2">
         <v>8.0</v>
@@ -1941,27 +1957,27 @@
         <v>80.0</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L33" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C34" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G34" s="2">
         <v>5.0</v>
@@ -1976,10 +1992,10 @@
         <v>75.0</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>30</v>
@@ -1987,16 +2003,16 @@
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G35" s="2">
         <v>8.0</v>
@@ -2011,27 +2027,27 @@
         <v>75.0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C36" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G36" s="2">
         <v>8.0</v>
@@ -2046,27 +2062,27 @@
         <v>80.0</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G37" s="2">
         <v>7.0</v>
@@ -2081,27 +2097,27 @@
         <v>75.0</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E38" s="2">
         <v>4.0</v>
@@ -2115,7 +2131,7 @@
         <v>75.0</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L38" s="2" t="s">
         <v>34</v>
@@ -2126,16 +2142,16 @@
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G39" s="2">
         <v>9.0</v>
@@ -2150,27 +2166,27 @@
         <v>70.0</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L39" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C40" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G40" s="2">
         <v>10.0</v>
@@ -2185,27 +2201,27 @@
         <v>75.0</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G41" s="2">
         <v>10.0</v>
@@ -2220,27 +2236,27 @@
         <v>80.0</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C42" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G42" s="2">
         <v>8.0</v>
@@ -2255,27 +2271,27 @@
         <v>80.0</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G43" s="2">
         <v>9.0</v>
@@ -2290,27 +2306,27 @@
         <v>80.0</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C44" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G44" s="2">
         <v>8.0</v>
@@ -2325,27 +2341,27 @@
         <v>80.0</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C45" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G45" s="2">
         <v>12.0</v>
@@ -2360,10 +2376,10 @@
         <v>70.0</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>30</v>
@@ -2377,21 +2393,21 @@
     <row r="49" ht="12.75" customHeight="1"/>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C51" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E51" s="2">
         <v>5.0</v>
@@ -2404,7 +2420,7 @@
         <v>75.0</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L51" s="1" t="str">
         <f>L20</f>
@@ -2417,16 +2433,16 @@
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E52" s="2">
         <v>2.0</v>
@@ -2439,7 +2455,7 @@
         <v>73.0</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L52" s="1" t="str">
         <f>L20</f>
@@ -2450,21 +2466,21 @@
         <v/>
       </c>
       <c r="N52" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C53" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E53" s="2">
         <v>30.0</v>
@@ -2477,7 +2493,7 @@
         <v>90.0</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L53" s="1" t="str">
         <f>L4&amp;L5&amp;L9</f>
@@ -2488,21 +2504,21 @@
         <v>BraçCamaTors</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C54" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G54" s="2">
         <v>20.0</v>
@@ -2517,7 +2533,7 @@
         <v>80.0</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L54" s="1" t="str">
         <f>L4&amp;L5&amp;L7</f>
@@ -2529,21 +2545,21 @@
       </c>
       <c r="N54" s="1" t="str">
         <f>N4&amp;N10&amp;N6</f>
-        <v>Baixar_de_pesManteniment</v>
+        <v>Baixar_de_pesYogaManteniment</v>
       </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C55" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G55" s="2">
         <v>6.0</v>
@@ -2558,7 +2574,7 @@
         <v>75.0</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L55" s="1" t="str">
         <f>L5</f>
@@ -2571,16 +2587,16 @@
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C56" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G56" s="2">
         <v>10.0</v>
@@ -2595,7 +2611,7 @@
         <v>65.0</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L56" s="1" t="str">
         <f>L9&amp;L4</f>
@@ -2608,16 +2624,16 @@
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C57" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E57" s="2">
         <v>10.0</v>
@@ -2630,7 +2646,7 @@
         <v>85.0</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L57" s="1" t="str">
         <f>L5</f>
@@ -2647,16 +2663,16 @@
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C58" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E58" s="2">
         <v>10.0</v>
@@ -2669,27 +2685,27 @@
         <v>85.0</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L58" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C59" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E59" s="2">
         <v>10.0</v>
@@ -2702,27 +2718,27 @@
         <v>85.0</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" ht="12.75" customHeight="1">
       <c r="A60" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C60" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E60" s="2">
         <v>2.0</v>
@@ -2735,7 +2751,7 @@
         <v>80.0</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L60" s="1" t="str">
         <f>L7&amp;L4&amp;L6</f>
@@ -2745,21 +2761,21 @@
         <v>29</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C61" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E61" s="2">
         <v>1.0</v>
@@ -2772,7 +2788,7 @@
         <v>75.0</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L61" s="2" t="s">
         <v>25</v>
@@ -2783,16 +2799,16 @@
     </row>
     <row r="62" ht="12.75" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C62" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E62" s="2">
         <v>1.0</v>
@@ -2805,27 +2821,27 @@
         <v>65.0</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L62" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>24</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" ht="12.75" customHeight="1">
       <c r="A63" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C63" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G63" s="2">
         <v>6.0</v>
@@ -2840,27 +2856,27 @@
         <v>75.0</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" ht="12.75" customHeight="1">
       <c r="A64" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C64" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G64" s="2">
         <v>5.0</v>
@@ -2875,27 +2891,27 @@
         <v>80.0</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L64" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C65" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G65" s="2">
         <v>6.0</v>
@@ -2910,7 +2926,7 @@
         <v>70.0</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L65" s="2" t="s">
         <v>34</v>
@@ -2921,16 +2937,16 @@
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C66" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G66" s="2">
         <v>6.0</v>
@@ -2945,27 +2961,27 @@
         <v>70.0</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L66" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C67" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G67" s="2">
         <v>6.0</v>
@@ -2980,27 +2996,27 @@
         <v>70.0</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C68" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G68" s="2">
         <v>5.0</v>
@@ -3015,27 +3031,27 @@
         <v>70.0</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L68" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C69" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E69" s="2">
         <v>4.0</v>
@@ -3048,7 +3064,7 @@
         <v>65.0</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L69" s="2" t="s">
         <v>34</v>
@@ -3059,16 +3075,16 @@
     </row>
     <row r="70" ht="12.75" customHeight="1">
       <c r="A70" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C70" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E70" s="2">
         <v>4.0</v>
@@ -3081,27 +3097,27 @@
         <v>70.0</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="N70" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C71" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E71" s="2">
         <v>4.0</v>
@@ -3114,7 +3130,7 @@
         <v>70.0</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L71" s="2" t="s">
         <v>25</v>
@@ -3125,16 +3141,16 @@
     </row>
     <row r="72" ht="12.75" customHeight="1">
       <c r="A72" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C72" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E72" s="2">
         <v>4.0</v>
@@ -3147,27 +3163,27 @@
         <v>70.0</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L72" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="A73" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C73" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G73" s="2">
         <v>6.0</v>
@@ -3182,7 +3198,7 @@
         <v>80.0</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>23</v>
@@ -3193,16 +3209,16 @@
     </row>
     <row r="74" ht="12.75" customHeight="1">
       <c r="A74" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C74" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E74" s="2">
         <v>3.0</v>
@@ -3215,7 +3231,7 @@
         <v>70.0</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L74" s="2" t="s">
         <v>34</v>
@@ -3226,16 +3242,16 @@
     </row>
     <row r="75" ht="12.75" customHeight="1">
       <c r="A75" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C75" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E75" s="2">
         <v>3.0</v>
@@ -3248,28 +3264,28 @@
         <v>80.0</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L75" s="1" t="str">
         <f>L4</f>
         <v>Braç</v>
       </c>
       <c r="N75" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" ht="12.75" customHeight="1">
       <c r="A76" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C76" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E76" s="2">
         <v>2.0</v>
@@ -3282,7 +3298,7 @@
         <v>70.0</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L76" s="2" t="s">
         <v>34</v>
@@ -3293,16 +3309,16 @@
     </row>
     <row r="77" ht="12.75" customHeight="1">
       <c r="A77" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C77" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E77" s="2">
         <v>3.0</v>
@@ -3315,27 +3331,27 @@
         <v>75.0</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" ht="12.75" customHeight="1">
       <c r="A78" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C78" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G78" s="2">
         <v>6.0</v>
@@ -3350,27 +3366,27 @@
         <v>75.0</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L78" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" ht="12.75" customHeight="1">
       <c r="A79" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C79" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E79" s="2">
         <v>3.0</v>
@@ -3383,10 +3399,10 @@
         <v>75.0</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="N79" s="2" t="s">
         <v>24</v>
@@ -3394,16 +3410,16 @@
     </row>
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C80" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E80" s="2">
         <v>5.0</v>
@@ -3416,27 +3432,27 @@
         <v>90.0</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L80" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" ht="12.75" customHeight="1">
       <c r="A81" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C81" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E81" s="2">
         <v>3.0</v>
@@ -3449,13 +3465,13 @@
         <v>75.0</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L81" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N81" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" ht="12.75" customHeight="1"/>
@@ -3463,21 +3479,21 @@
     <row r="84" ht="12.75" customHeight="1"/>
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" ht="12.75" customHeight="1">
       <c r="A86" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C86" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E86" s="2">
         <v>5.0</v>
@@ -3490,7 +3506,7 @@
         <v>85.0</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L86" s="2" t="s">
         <v>34</v>
@@ -3499,21 +3515,21 @@
         <v>34</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C87" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E87" s="2">
         <v>5.0</v>
@@ -3526,7 +3542,7 @@
         <v>80.0</v>
       </c>
       <c r="K87" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L87" s="2" t="s">
         <v>34</v>
@@ -3540,16 +3556,16 @@
     </row>
     <row r="88" ht="12.75" customHeight="1">
       <c r="A88" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E88" s="2">
         <v>3.0</v>
@@ -3562,7 +3578,7 @@
         <v>80.0</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L88" s="2" t="s">
         <v>27</v>
@@ -3571,21 +3587,21 @@
         <v>27</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>35</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" ht="12.75" customHeight="1">
       <c r="A89" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C89" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G89" s="2">
         <v>6.0</v>
@@ -3600,7 +3616,7 @@
         <v>75.0</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L89" s="2" t="s">
         <v>27</v>
@@ -3614,16 +3630,16 @@
     </row>
     <row r="90" ht="12.75" customHeight="1">
       <c r="A90" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C90" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G90" s="2">
         <v>6.0</v>
@@ -3638,7 +3654,7 @@
         <v>80.0</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L90" s="2" t="s">
         <v>27</v>
@@ -3652,16 +3668,16 @@
     </row>
     <row r="91" ht="12.75" customHeight="1">
       <c r="A91" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C91" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G91" s="2">
         <v>5.0</v>
@@ -3676,7 +3692,7 @@
         <v>80.0</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L91" s="2" t="s">
         <v>27</v>
@@ -3690,16 +3706,16 @@
     </row>
     <row r="92" ht="12.75" customHeight="1">
       <c r="A92" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C92" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G92" s="2">
         <v>5.0</v>
@@ -3714,7 +3730,7 @@
         <v>80.0</v>
       </c>
       <c r="K92" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L92" s="2" t="s">
         <v>27</v>
@@ -3728,16 +3744,16 @@
     </row>
     <row r="93" ht="12.75" customHeight="1">
       <c r="A93" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C93" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E93" s="2">
         <v>3.0</v>
@@ -3750,7 +3766,7 @@
         <v>75.0</v>
       </c>
       <c r="K93" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L93" s="2" t="s">
         <v>25</v>
@@ -3764,16 +3780,16 @@
     </row>
     <row r="94" ht="12.75" customHeight="1">
       <c r="A94" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C94" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E94" s="2">
         <v>5.0</v>
@@ -3786,7 +3802,7 @@
         <v>80.0</v>
       </c>
       <c r="K94" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L94" s="2" t="s">
         <v>25</v>
@@ -3800,16 +3816,16 @@
     </row>
     <row r="95" ht="12.75" customHeight="1">
       <c r="A95" s="3" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C95" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G95" s="2">
         <v>6.0</v>
@@ -3824,7 +3840,7 @@
         <v>75.0</v>
       </c>
       <c r="K95" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L95" s="2" t="s">
         <v>25</v>
@@ -3833,21 +3849,21 @@
         <v>25</v>
       </c>
       <c r="N95" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
     </row>
     <row r="96" ht="12.75" customHeight="1">
       <c r="A96" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="C96" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G96" s="2">
         <v>6.0</v>
@@ -3862,7 +3878,7 @@
         <v>80.0</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L96" s="2" t="s">
         <v>25</v>
@@ -3876,16 +3892,16 @@
     </row>
     <row r="97" ht="12.75" customHeight="1">
       <c r="A97" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C97" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G97" s="2">
         <v>5.0</v>
@@ -3900,7 +3916,7 @@
         <v>80.0</v>
       </c>
       <c r="K97" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L97" s="2" t="s">
         <v>25</v>
@@ -3914,16 +3930,16 @@
     </row>
     <row r="98" ht="12.75" customHeight="1">
       <c r="A98" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C98" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E98" s="2">
         <v>3.0</v>
@@ -3935,7 +3951,7 @@
         <v>75.0</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L98" s="2" t="s">
         <v>34</v>
@@ -3944,21 +3960,21 @@
         <v>34</v>
       </c>
       <c r="N98" s="2" t="s">
-        <v>35</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" ht="12.75" customHeight="1">
       <c r="A99" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C99" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G99" s="2">
         <v>6.0</v>
@@ -3973,7 +3989,7 @@
         <v>80.0</v>
       </c>
       <c r="K99" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L99" s="2" t="s">
         <v>25</v>
@@ -3987,16 +4003,16 @@
     </row>
     <row r="100" ht="12.75" customHeight="1">
       <c r="A100" s="3" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="C100" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E100" s="2">
         <v>3.0</v>
@@ -4009,7 +4025,7 @@
         <v>80.0</v>
       </c>
       <c r="K100" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L100" s="2" t="s">
         <v>34</v>
@@ -4023,16 +4039,16 @@
     </row>
     <row r="101" ht="12.75" customHeight="1">
       <c r="A101" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="C101" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E101" s="2">
         <v>3.0</v>
@@ -4045,7 +4061,7 @@
         <v>75.0</v>
       </c>
       <c r="K101" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L101" s="2" t="s">
         <v>31</v>
@@ -4059,16 +4075,16 @@
     </row>
     <row r="102" ht="12.75" customHeight="1">
       <c r="A102" s="3" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C102" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E102" s="2">
         <v>4.0</v>
@@ -4081,7 +4097,7 @@
         <v>80.0</v>
       </c>
       <c r="K102" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L102" s="2" t="s">
         <v>23</v>
@@ -4095,16 +4111,16 @@
     </row>
     <row r="103" ht="12.75" customHeight="1">
       <c r="A103" s="3" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C103" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E103" s="2">
         <v>4.0</v>
@@ -4117,7 +4133,7 @@
         <v>80.0</v>
       </c>
       <c r="K103" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L103" s="2" t="s">
         <v>23</v>
@@ -4131,16 +4147,16 @@
     </row>
     <row r="104" ht="12.75" customHeight="1">
       <c r="A104" s="3" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C104" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E104" s="2">
         <v>4.0</v>
@@ -4153,7 +4169,7 @@
         <v>75.0</v>
       </c>
       <c r="K104" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L104" s="2" t="s">
         <v>29</v>
@@ -4162,21 +4178,21 @@
         <v>29</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
     </row>
     <row r="105" ht="12.75" customHeight="1">
       <c r="A105" s="3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="C105" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G105" s="2">
         <v>10.0</v>
@@ -4191,7 +4207,7 @@
         <v>75.0</v>
       </c>
       <c r="K105" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L105" s="2" t="s">
         <v>29</v>
@@ -4205,16 +4221,16 @@
     </row>
     <row r="106" ht="12.75" customHeight="1">
       <c r="A106" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="C106" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G106" s="2">
         <v>8.0</v>
@@ -4229,7 +4245,7 @@
         <v>75.0</v>
       </c>
       <c r="K106" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L106" s="2" t="s">
         <v>34</v>
@@ -4243,16 +4259,16 @@
     </row>
     <row r="107" ht="12.75" customHeight="1">
       <c r="A107" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C107" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E107" s="2">
         <v>20.0</v>
@@ -4265,37 +4281,37 @@
         <v>80.0</v>
       </c>
       <c r="K107" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L107" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="M107" s="2" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="N107" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
     </row>
     <row r="108" ht="12.75" customHeight="1"/>
     <row r="109" ht="12.75" customHeight="1"/>
     <row r="110" ht="12.75" customHeight="1">
       <c r="A110" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" ht="12.75" customHeight="1">
       <c r="A111" s="2" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C111" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E111" s="2">
         <v>3.0</v>
@@ -4308,27 +4324,27 @@
         <v>80.0</v>
       </c>
       <c r="K111" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L111" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" ht="12.75" customHeight="1">
       <c r="A112" s="5" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C112" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E112" s="2">
         <v>4.0</v>
@@ -4341,27 +4357,27 @@
         <v>80.0</v>
       </c>
       <c r="K112" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L112" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" ht="12.75" customHeight="1">
       <c r="A113" s="5" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="C113" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E113" s="2">
         <v>4.0</v>
@@ -4374,27 +4390,27 @@
         <v>80.0</v>
       </c>
       <c r="K113" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L113" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N113" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" ht="12.75" customHeight="1">
       <c r="A114" s="5" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C114" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E114" s="2">
         <v>4.0</v>
@@ -4407,27 +4423,27 @@
         <v>80.0</v>
       </c>
       <c r="K114" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L114" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="115" ht="12.75" customHeight="1">
       <c r="A115" s="5" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="C115" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E115" s="2">
         <v>4.0</v>
@@ -4440,27 +4456,27 @@
         <v>80.0</v>
       </c>
       <c r="K115" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L115" s="2" t="s">
         <v>27</v>
       </c>
       <c r="N115" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="116" ht="12.75" customHeight="1">
       <c r="A116" s="5" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C116" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E116" s="2">
         <v>4.0</v>
@@ -4473,27 +4489,27 @@
         <v>80.0</v>
       </c>
       <c r="K116" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L116" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="117" ht="12.75" customHeight="1">
       <c r="A117" s="5" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="C117" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E117" s="2">
         <v>5.0</v>
@@ -4506,27 +4522,27 @@
         <v>80.0</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L117" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N117" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="118" ht="12.75" customHeight="1">
       <c r="A118" s="5" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C118" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E118" s="2">
         <v>3.0</v>
@@ -4539,60 +4555,59 @@
         <v>80.0</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L118" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N118" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="119" ht="12.75" customHeight="1">
       <c r="A119" s="2" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C119" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E119" s="2">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="F119" s="2">
         <v>7.0</v>
       </c>
-      <c r="G119" s="2"/>
       <c r="J119" s="2">
-        <v>80.0</v>
+        <v>65.0</v>
       </c>
       <c r="K119" s="2" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="L119" s="2" t="s">
-        <v>29</v>
+        <v>239</v>
       </c>
       <c r="N119" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" ht="12.75" customHeight="1">
       <c r="A120" s="2" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="C120" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E120" s="2">
         <v>7.0</v>
@@ -4604,7 +4619,7 @@
         <v>75.0</v>
       </c>
       <c r="K120" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L120" s="2" t="s">
         <v>29</v>
@@ -4613,21 +4628,21 @@
         <v>29</v>
       </c>
       <c r="N120" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="121" ht="12.75" customHeight="1">
       <c r="A121" s="2" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="C121" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E121" s="2">
         <v>6.0</v>
@@ -4639,27 +4654,27 @@
         <v>75.0</v>
       </c>
       <c r="K121" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L121" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N121" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="122" ht="12.75" customHeight="1">
       <c r="A122" s="2" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C122" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E122" s="2">
         <v>7.0</v>
@@ -4671,27 +4686,27 @@
         <v>80.0</v>
       </c>
       <c r="K122" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="N122" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="123" ht="12.75" customHeight="1">
       <c r="A123" s="2" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="C123" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E123" s="2">
         <v>8.0</v>
@@ -4703,27 +4718,27 @@
         <v>80.0</v>
       </c>
       <c r="K123" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L123" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N123" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" ht="12.75" customHeight="1">
       <c r="A124" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C124" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E124" s="2">
         <v>6.0</v>
@@ -4735,27 +4750,27 @@
         <v>75.0</v>
       </c>
       <c r="K124" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>26</v>
+        <v>222</v>
       </c>
     </row>
     <row r="125" ht="12.75" customHeight="1">
       <c r="A125" s="2" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C125" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E125" s="2">
         <v>7.0</v>
@@ -4767,47 +4782,16 @@
         <v>70.0</v>
       </c>
       <c r="K125" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="126" ht="12.75" customHeight="1">
-      <c r="A126" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C126" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E126" s="2">
-        <v>6.0</v>
-      </c>
-      <c r="F126" s="2">
-        <v>7.0</v>
-      </c>
-      <c r="J126" s="2">
-        <v>65.0</v>
-      </c>
-      <c r="K126" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L126" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="N126" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="126" ht="12.75" customHeight="1"/>
     <row r="127" ht="12.75" customHeight="1"/>
     <row r="128" ht="12.75" customHeight="1"/>
     <row r="129" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
actualitzar ontologia i comentarla
</commit_message>
<xml_diff>
--- a/exercices_to_clips/exercicisExcel.xlsx
+++ b/exercices_to_clips/exercicisExcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="252">
   <si>
     <t>nom_instancia</t>
   </si>
@@ -760,6 +760,9 @@
   </si>
   <si>
     <t>estiramiento_de_isquiotibiales_en_pie</t>
+  </si>
+  <si>
+    <t>estiramiento de isquiotibiales en pie</t>
   </si>
   <si>
     <t>estiramiento triceps</t>
@@ -4700,7 +4703,7 @@
         <v>247</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C123" s="2" t="b">
         <v>0</v>
@@ -4732,7 +4735,7 @@
         <v>208</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C124" s="2" t="b">
         <v>0</v>
@@ -4761,10 +4764,10 @@
     </row>
     <row r="125" ht="12.75" customHeight="1">
       <c r="A125" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C125" s="2" t="b">
         <v>0</v>

</xml_diff>